<commit_message>
Separate artist and album list in the wireframes
</commit_message>
<xml_diff>
--- a/wireframes/Example Data.xlsx
+++ b/wireframes/Example Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MusicCatalogue\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A1D4F7-9D99-4C6A-A5B8-8E4A7776AA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED45434-8C97-43FD-9F2C-CE989E24A2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="1" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" activeTab="2" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Albums" sheetId="1" r:id="rId1"/>
-    <sheet name="Tracks" sheetId="3" r:id="rId2"/>
+    <sheet name="Artists" sheetId="4" r:id="rId1"/>
+    <sheet name="Albums" sheetId="1" r:id="rId2"/>
+    <sheet name="Tracks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,26 +38,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
-  <si>
-    <t>Blue Train</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>John Coltrane</t>
   </si>
   <si>
-    <t>Jazz</t>
-  </si>
-  <si>
-    <t>Brothers in Arms</t>
-  </si>
-  <si>
     <t>Dire Straits</t>
   </si>
   <si>
-    <t>Rock</t>
-  </si>
-  <si>
     <t>Let It Be</t>
   </si>
   <si>
@@ -66,15 +55,9 @@
     <t>Rock &amp; Roll</t>
   </si>
   <si>
-    <t>Royal Blues</t>
-  </si>
-  <si>
     <t>Dragonette</t>
   </si>
   <si>
-    <t>Dance</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -90,18 +73,6 @@
     <t>CoverUrl</t>
   </si>
   <si>
-    <t>Moment's Notice</t>
-  </si>
-  <si>
-    <t>Locomotion</t>
-  </si>
-  <si>
-    <t>I'm Old Fashioned</t>
-  </si>
-  <si>
-    <t>Lazy Bird</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -115,6 +86,57 @@
   </si>
   <si>
     <t>Track</t>
+  </si>
+  <si>
+    <t>Back In The U.S.S.R.</t>
+  </si>
+  <si>
+    <t>Dear Prudence</t>
+  </si>
+  <si>
+    <t>Glass Onion</t>
+  </si>
+  <si>
+    <t>Ob-La-Di, Ob-La-Da</t>
+  </si>
+  <si>
+    <t>Wild Honey Pie</t>
+  </si>
+  <si>
+    <t>The Continuing Story Of Bungalow Bill</t>
+  </si>
+  <si>
+    <t>While My Guitar Gently Weeps</t>
+  </si>
+  <si>
+    <t>Happiness Is A Warm Gun</t>
+  </si>
+  <si>
+    <t>Martha My Dear</t>
+  </si>
+  <si>
+    <t>I'm So Tired</t>
+  </si>
+  <si>
+    <t>Blackbird</t>
+  </si>
+  <si>
+    <t>Piggies</t>
+  </si>
+  <si>
+    <t>Rocky Raccoon</t>
+  </si>
+  <si>
+    <t>Don't Pass Me By</t>
+  </si>
+  <si>
+    <t>Why Don't We Do It In The Road?</t>
+  </si>
+  <si>
+    <t>I Will</t>
+  </si>
+  <si>
+    <t>Julia</t>
   </si>
 </sst>
 </file>
@@ -483,12 +505,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EAF001-090A-4684-B0C3-A5E29071EADF}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.46484375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96989E08-D66E-4965-A794-B1EEDF85B06F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -502,36 +566,36 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1957</v>
+        <v>1970</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -539,67 +603,16 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3">
-        <v>1985</v>
+        <v>1968</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>1970</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>2016</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>1968</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -607,9 +620,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982CFB61-704D-42D9-978A-3C5B633D04BA}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -618,54 +631,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.46484375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.86328125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3">
-        <v>0.4465277777777778</v>
+        <v>0.11319444444444444</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -674,15 +687,15 @@
         <v>17</v>
       </c>
       <c r="E3" s="3">
-        <v>0.38194444444444442</v>
+        <v>0.16388888888888889</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -691,15 +704,15 @@
         <v>18</v>
       </c>
       <c r="E4" s="3">
-        <v>0.30138888888888887</v>
+        <v>9.5138888888888884E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -708,15 +721,15 @@
         <v>19</v>
       </c>
       <c r="E5" s="3">
-        <v>0.33194444444444443</v>
+        <v>0.13055555555555556</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -725,7 +738,211 @@
         <v>20</v>
       </c>
       <c r="E6" s="3">
-        <v>0.2951388888888889</v>
+        <v>3.6111111111111115E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.13472222222222222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.19791666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.11319444444444444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.10277777777777779</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8.5416666666666655E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="3">
+        <v>9.5833333333333326E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8.6111111111111124E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.14722222222222223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.15972222222222224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7.013888888888889E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7.3611111111111113E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.12083333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add album/track stats to artists page in wireframes
</commit_message>
<xml_diff>
--- a/wireframes/Example Data.xlsx
+++ b/wireframes/Example Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MusicCatalogue\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED45434-8C97-43FD-9F2C-CE989E24A2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D2C63F-4CBC-4FAB-ABDD-06025415B2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="14235" activeTab="2" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Artists" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>John Coltrane</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>Julia</t>
+  </si>
+  <si>
+    <t>Albums</t>
+  </si>
+  <si>
+    <t>Tracks</t>
   </si>
 </sst>
 </file>
@@ -506,38 +512,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EAF001-090A-4684-B0C3-A5E29071EADF}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>3</v>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -624,9 +663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982CFB61-704D-42D9-978A-3C5B633D04BA}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Completed UI for the job status report
</commit_message>
<xml_diff>
--- a/wireframes/Example Data.xlsx
+++ b/wireframes/Example Data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MusicCatalogue\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D2C63F-4CBC-4FAB-ABDD-06025415B2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7594B4C8-DB9B-46FA-99AF-661CF40D9404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Artists" sheetId="4" r:id="rId1"/>
     <sheet name="Albums" sheetId="1" r:id="rId2"/>
     <sheet name="Tracks" sheetId="3" r:id="rId3"/>
+    <sheet name="Job Status" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
   <si>
     <t>John Coltrane</t>
   </si>
@@ -143,12 +144,36 @@
   </si>
   <si>
     <t>Tracks</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Catalogue Export</t>
+  </si>
+  <si>
+    <t>JobName = Catalogue Export, FileName = Example.csv</t>
+  </si>
+  <si>
+    <t>JobName = Catalogue Export, FileName = 2023-10-29 Export.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -198,6 +223,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EAF001-090A-4684-B0C3-A5E29071EADF}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -987,4 +1014,85 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F68ACC-B50B-49DB-A71B-07EF183484E9}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="6">
+        <v>45228.5255921875</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45228.525594918981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6">
+        <v>45228.530457615743</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45228.530460266207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="6">
+        <v>45228.684753900459</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45228.684756863426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated README to include Wish List
</commit_message>
<xml_diff>
--- a/wireframes/Example Data.xlsx
+++ b/wireframes/Example Data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MusicCatalogue\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7594B4C8-DB9B-46FA-99AF-661CF40D9404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF98D71-9546-450C-A5E6-7A0D83240462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="3" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
+    <workbookView xWindow="907" yWindow="2422" windowWidth="14483" windowHeight="9983" activeTab="4" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Artists" sheetId="4" r:id="rId1"/>
     <sheet name="Albums" sheetId="1" r:id="rId2"/>
     <sheet name="Tracks" sheetId="3" r:id="rId3"/>
     <sheet name="Job Status" sheetId="5" r:id="rId4"/>
+    <sheet name="Wish List Track List" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
   <si>
     <t>John Coltrane</t>
   </si>
@@ -165,6 +166,48 @@
   </si>
   <si>
     <t>JobName = Catalogue Export, FileName = 2023-10-29 Export.csv</t>
+  </si>
+  <si>
+    <t>Live In Paris</t>
+  </si>
+  <si>
+    <t>Diana Krall</t>
+  </si>
+  <si>
+    <t>I Love Being Here With You</t>
+  </si>
+  <si>
+    <t>Let's Fall In Love</t>
+  </si>
+  <si>
+    <t>'Deed I Do</t>
+  </si>
+  <si>
+    <t>The Look Of Love</t>
+  </si>
+  <si>
+    <t>East Of The Sun (And West Of The Moon)</t>
+  </si>
+  <si>
+    <t>I've Got You Under My Skin</t>
+  </si>
+  <si>
+    <t>Devil May Care</t>
+  </si>
+  <si>
+    <t>Maybe You'll Be There</t>
+  </si>
+  <si>
+    <t>'S Wonderful</t>
+  </si>
+  <si>
+    <t>Fly Me To The Moon</t>
+  </si>
+  <si>
+    <t>A Case Of You</t>
+  </si>
+  <si>
+    <t>Just The Way You Are</t>
   </si>
 </sst>
 </file>
@@ -692,7 +735,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1020,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F68ACC-B50B-49DB-A71B-07EF183484E9}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -1095,4 +1138,261 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6940BD2-0C04-446D-AD3E-285BA0B180B6}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.46484375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.53125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.21666666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.19027777777777777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.22013888888888888</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.24861111111111112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.30833333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.28611111111111115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.24097222222222223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.24930555555555556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.25347222222222221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.29444444444444445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added purchase details to the wireframes
</commit_message>
<xml_diff>
--- a/wireframes/Example Data.xlsx
+++ b/wireframes/Example Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MusicCatalogue\wireframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF98D71-9546-450C-A5E6-7A0D83240462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE89EBA-01DD-491A-BC51-50463097639D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="907" yWindow="2422" windowWidth="14483" windowHeight="9983" activeTab="4" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{15DD7874-E3AC-48B4-91FA-AD958DB02DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Artists" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
   <si>
     <t>John Coltrane</t>
   </si>
@@ -72,15 +72,9 @@
     <t>Released</t>
   </si>
   <si>
-    <t>CoverUrl</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
-    <t>Cover</t>
-  </si>
-  <si>
     <t>Album</t>
   </si>
   <si>
@@ -208,13 +202,29 @@
   </si>
   <si>
     <t>Just The Way You Are</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Purchased</t>
+  </si>
+  <si>
+    <t>Retailer</t>
+  </si>
+  <si>
+    <t>HMV</t>
+  </si>
+  <si>
+    <t>Dig Vinyl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -254,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -268,6 +278,11 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EAF001-090A-4684-B0C3-A5E29071EADF}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -594,18 +609,21 @@
     <col min="2" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -615,8 +633,11 @@
       <c r="C2" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -626,8 +647,11 @@
       <c r="C3" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -637,8 +661,11 @@
       <c r="C4" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -647,6 +674,9 @@
       </c>
       <c r="C5" s="2">
         <v>29</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -657,7 +687,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96989E08-D66E-4965-A794-B1EEDF85B06F}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -670,10 +700,10 @@
     <col min="2" max="2" width="11.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.73046875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -687,10 +717,16 @@
         <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -703,11 +739,17 @@
       <c r="D2">
         <v>1970</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E2" s="8">
+        <v>44927</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -720,8 +762,14 @@
       <c r="D3">
         <v>1968</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="E3" s="8">
+        <v>44927</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -750,19 +798,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -776,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3">
         <v>0.11319444444444444</v>
@@ -793,7 +841,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3">
         <v>0.16388888888888889</v>
@@ -810,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="3">
         <v>9.5138888888888884E-2</v>
@@ -827,7 +875,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3">
         <v>0.13055555555555556</v>
@@ -844,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3">
         <v>3.6111111111111115E-2</v>
@@ -861,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3">
         <v>0.13472222222222222</v>
@@ -878,7 +926,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="3">
         <v>0.19791666666666666</v>
@@ -895,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3">
         <v>0.11319444444444444</v>
@@ -912,7 +960,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3">
         <v>0.10277777777777779</v>
@@ -929,7 +977,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="3">
         <v>8.5416666666666655E-2</v>
@@ -946,7 +994,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="3">
         <v>9.5833333333333326E-2</v>
@@ -963,7 +1011,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3">
         <v>8.6111111111111124E-2</v>
@@ -980,7 +1028,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3">
         <v>0.14722222222222223</v>
@@ -997,7 +1045,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3">
         <v>0.15972222222222224</v>
@@ -1014,7 +1062,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3">
         <v>7.013888888888889E-2</v>
@@ -1031,7 +1079,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3">
         <v>7.3611111111111113E-2</v>
@@ -1048,7 +1096,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E18" s="3">
         <v>0.12083333333333333</v>
@@ -1081,24 +1129,24 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="6">
         <v>45228.5255921875</v>
@@ -1109,10 +1157,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6">
         <v>45228.530457615743</v>
@@ -1123,10 +1171,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
         <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
       </c>
       <c r="C4" s="6">
         <v>45228.684753900459</v>
@@ -1144,7 +1192,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6940BD2-0C04-446D-AD3E-285BA0B180B6}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1158,33 +1209,33 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3">
         <v>0.21666666666666667</v>
@@ -1192,16 +1243,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E3" s="3">
         <v>0.19027777777777777</v>
@@ -1209,16 +1260,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="3">
         <v>0.22013888888888888</v>
@@ -1226,16 +1277,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="3">
         <v>0.20833333333333334</v>
@@ -1243,16 +1294,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6" s="3">
         <v>0.24861111111111112</v>
@@ -1260,16 +1311,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3">
         <v>0.30833333333333335</v>
@@ -1277,16 +1328,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="3">
         <v>0.28611111111111115</v>
@@ -1294,16 +1345,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E9" s="3">
         <v>0.24097222222222223</v>
@@ -1311,16 +1362,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="3">
         <v>0.24930555555555556</v>
@@ -1328,16 +1379,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="3">
         <v>0.25347222222222221</v>
@@ -1345,16 +1396,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="2">
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3">
         <v>0.29444444444444445</v>
@@ -1362,16 +1413,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2">
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="3">
         <v>0.20833333333333334</v>

</xml_diff>